<commit_message>
Graduate Data Email Merge
</commit_message>
<xml_diff>
--- a/PHS_Grade12@psd1.org.xlsx
+++ b/PHS_Grade12@psd1.org.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John C. Weisenfeld\Documents\GitHub\Misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{FED3F62E-B884-4DF6-91A9-8F76FF29F5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{79EF6000-EC1E-4FD5-A846-F8D3DE50F8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="855" yWindow="-120" windowWidth="19755" windowHeight="11760"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5079" uniqueCount="2443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5079" uniqueCount="2442">
   <si>
     <t>ExtensionData</t>
   </si>
@@ -7271,9 +7271,6 @@
   </si>
   <si>
     <t>Adriana</t>
-  </si>
-  <si>
-    <t>Zu?iga</t>
   </si>
   <si>
     <t>Gradaille</t>
@@ -8193,8 +8190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O545"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H514" workbookViewId="0">
-      <selection activeCell="J520" sqref="J520"/>
+    <sheetView tabSelected="1" topLeftCell="H184" workbookViewId="0">
+      <selection activeCell="L505" sqref="L505"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8245,19 +8242,19 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>2437</v>
+      </c>
+      <c r="L1" t="s">
         <v>2438</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>2439</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>2440</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>2441</v>
-      </c>
-      <c r="O1" t="s">
-        <v>2442</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -26365,7 +26362,7 @@
         <v>16</v>
       </c>
       <c r="K505" t="s">
-        <v>1525</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="506" spans="1:15" x14ac:dyDescent="0.25">
@@ -27197,7 +27194,7 @@
         <v>2143</v>
       </c>
       <c r="M528" t="s">
-        <v>2417</v>
+        <v>2238</v>
       </c>
     </row>
     <row r="529" spans="1:13" x14ac:dyDescent="0.25">
@@ -27232,7 +27229,7 @@
         <v>1686</v>
       </c>
       <c r="L529" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
     </row>
     <row r="530" spans="1:13" x14ac:dyDescent="0.25">
@@ -27267,7 +27264,7 @@
         <v>2399</v>
       </c>
       <c r="L530" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
     </row>
     <row r="531" spans="1:13" x14ac:dyDescent="0.25">
@@ -27299,10 +27296,10 @@
         <v>16</v>
       </c>
       <c r="K531" t="s">
+        <v>2419</v>
+      </c>
+      <c r="L531" t="s">
         <v>2420</v>
-      </c>
-      <c r="L531" t="s">
-        <v>2421</v>
       </c>
     </row>
     <row r="532" spans="1:13" x14ac:dyDescent="0.25">
@@ -27334,7 +27331,7 @@
         <v>16</v>
       </c>
       <c r="K532" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="L532" t="s">
         <v>1856</v>
@@ -27369,10 +27366,10 @@
         <v>16</v>
       </c>
       <c r="K533" t="s">
+        <v>2422</v>
+      </c>
+      <c r="L533" t="s">
         <v>2423</v>
-      </c>
-      <c r="L533" t="s">
-        <v>2424</v>
       </c>
     </row>
     <row r="534" spans="1:13" x14ac:dyDescent="0.25">
@@ -27404,10 +27401,10 @@
         <v>16</v>
       </c>
       <c r="K534" t="s">
+        <v>2424</v>
+      </c>
+      <c r="L534" t="s">
         <v>2425</v>
-      </c>
-      <c r="L534" t="s">
-        <v>2426</v>
       </c>
       <c r="M534" t="s">
         <v>1965</v>
@@ -27477,7 +27474,7 @@
         <v>16</v>
       </c>
       <c r="K536" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="L536" t="s">
         <v>1972</v>
@@ -27512,10 +27509,10 @@
         <v>16</v>
       </c>
       <c r="K537" t="s">
+        <v>2427</v>
+      </c>
+      <c r="L537" t="s">
         <v>2428</v>
-      </c>
-      <c r="L537" t="s">
-        <v>2429</v>
       </c>
       <c r="M537" t="s">
         <v>1657</v>
@@ -27550,10 +27547,10 @@
         <v>16</v>
       </c>
       <c r="K538" t="s">
+        <v>2429</v>
+      </c>
+      <c r="L538" t="s">
         <v>2430</v>
-      </c>
-      <c r="L538" t="s">
-        <v>2431</v>
       </c>
     </row>
     <row r="539" spans="1:13" x14ac:dyDescent="0.25">
@@ -27585,13 +27582,13 @@
         <v>16</v>
       </c>
       <c r="K539" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="L539" t="s">
         <v>2255</v>
       </c>
       <c r="M539" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
     </row>
     <row r="540" spans="1:13" x14ac:dyDescent="0.25">
@@ -27623,7 +27620,7 @@
         <v>16</v>
       </c>
       <c r="K540" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="L540" t="s">
         <v>1664</v>
@@ -27658,7 +27655,7 @@
         <v>16</v>
       </c>
       <c r="K541" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="L541" t="s">
         <v>2126</v>
@@ -27731,7 +27728,7 @@
         <v>1714</v>
       </c>
       <c r="L543" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="544" spans="1:13" x14ac:dyDescent="0.25">
@@ -27798,7 +27795,7 @@
         <v>16</v>
       </c>
       <c r="K545" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="L545" t="s">
         <v>1757</v>

</xml_diff>